<commit_message>
generated excel file appending all resume details.
</commit_message>
<xml_diff>
--- a/parsed_resumes.xlsx
+++ b/parsed_resumes.xlsx
@@ -1,117 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Resume Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>Year Of Study</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>Discipline</t>
-  </si>
-  <si>
-    <t>CGPA</t>
-  </si>
-  <si>
-    <t>Key Skills</t>
-  </si>
-  <si>
-    <t>Gen-AI Experience Score</t>
-  </si>
-  <si>
-    <t>AI/ML Experience Score</t>
-  </si>
-  <si>
-    <t>Overall Score</t>
-  </si>
-  <si>
-    <t>Supporting Information</t>
-  </si>
-  <si>
-    <t>Suggestions for improvement</t>
-  </si>
-  <si>
-    <t>SYED SADIQU HUSSAIN</t>
-  </si>
-  <si>
-    <t>syedsadiquh@gmail.com</t>
-  </si>
-  <si>
-    <t>+91-7846821811</t>
-  </si>
-  <si>
-    <t>Gandhi Institute for Technology (GIFT)</t>
-  </si>
-  <si>
-    <t>2022-2026</t>
-  </si>
-  <si>
-    <t>Bachelor of Technology in Computer Science Engineering (B.Tech)</t>
-  </si>
-  <si>
-    <t>Computer Science Engineering</t>
-  </si>
-  <si>
-    <t>8.24</t>
-  </si>
-  <si>
-    <t>Java, Python, FastAPI, Swing, Flask, Streamlit, Linux, Git, GitHub, MySQL</t>
-  </si>
-  <si>
-    <t>Flutter App Development Intern at London School of Digital Business, Embedded System Analyst at SDI-B, Project: LSDB Android Application, Project: Liquid Level Monitoring System, Task Manager with Priority, Geo-coding Application, Elite + Silver Certificate in NPTEL 'Programming, Data Structures, and Algorithms using Python', First position in 'Byte Rush' coding competition.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -145,16 +69,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -442,113 +433,412 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="65.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
-    <col min="9" max="9" width="75.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="379.7109375" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" customWidth="1"/>
+    <col width="29" customWidth="1" min="1" max="2"/>
+    <col width="53" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="58" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="66" customWidth="1" min="6" max="6"/>
+    <col width="34" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
+    <col width="228" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="24" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="347" customWidth="1" min="13" max="13"/>
+    <col width="29" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>University</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Year Of Study</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Course</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Discipline</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CGPA</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Key Skills</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Gen-AI Experience Score</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>AI/ML Experience Score</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Overall Score</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Supporting Information</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Suggestions for improvement</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MOHANTY HITESH RABINDRANATH</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mohantyhitesh4495@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>+916372773960</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gandhi Institute for Technology</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2022-2026</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology in Computer Science Engineering (B. Tech)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Computer Science Engineering</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>9+</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Python, C Programming, Data Structures &amp; Algorithms, Database Management System (DBMS), Core Java, Web Development, Java, JavaScript, C, SQL, HTML, CSS, MySQL, Git, Intellij Idea Ultimate, VS Code, NetBeans, TensorFlow, OpenCV</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Developed a Hospital Management System, Deep Text Recognizer with 70% accuracy, Java Development Intern at IIG Varsity, Elite Certificate in NPTEL Exam for Programming, Data Structure and Algorithm using Python, Second Position in Byte Rush: Coding Competition, Solved 60+ DSA Questions on Leetcode, Consistently Maintaining 9+ CGPA in Academics</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SYED SADIQU HUSSAIN</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>syedsadiquh@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>+91-7846821811</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Gandhi Institute for Technology (GIFT)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology in Computer Science Engineering (B.Tech)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Computer Science Engineering</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>8.24</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Java, Python, FastAPI, Swing, Flask, Streamlit, Linux, Git, GitHub, MySQL</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="K3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="L3" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Flutter App Development Intern at London School of Digital Business, Embedded System Analyst at SDI-B, Elite + Silver Certificate in NPTEL 'Programming, Data Structures, and Algorithms using Python', First position in 'Byte Rush' coding competition.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Abhisek Singh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>abhiseks2022@gift.edu.in, abhisekpsingh09@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>+91 6371007705</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Biju Patnaik University of Technology</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pursuing</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>B-Tech</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Computer Science and Engineering</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>7.95</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>HTML, CSS, Javascript, Python, C, Java, SQL, PowerPoint, MS Excel, MS Word, Visual Studios</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>1st prize in a general knowledge competition, Gold certificate in Big Data course from NASSCOM, Completed a hands-on Big Data workshop, Project: House Rental Management system using JAVA and SQL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ajnish Kumar</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ajnish2022@gift.edu.in / ajnishk4@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>+91 9693299625</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Gandhi Institute for Technology, Autonomous, Bhubaneswar</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pursuing</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>B. Tech</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Computer Science and Engineering</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>HTML, CSS, Tailwind CSS, React Js, Python, Java, JavaScript, Visual Studio Code, PyCharm, Git &amp; GitHub, Anaconda, SQL, MS Word, Excel, PowerPoint, DSA (Data Structure and Algorithm), Django</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Certified in Big Data Analytics from C-DAC, Completed an online Full Stack Development course from Apna College, Certification in Introduction to Cloud Computing from IIG Versity, Projects: Face-clone using Django, IoT-Based water level detector, Weather app</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Amit Kumar</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>kamit2022@gift.edu.in / amk373431@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>+91-7033010760</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Gandhi Institute for Technology (Autonomous)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>B.Tech</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Computer Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>8.5</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>HTML, CSS, JavaScript, C, C++, Python, SQL, Data Structures, Algorithms, Visual Studio Code, MS Word, Excel, PowerPoint</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0.33</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
+      <c r="L6" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Certificate by NPTEL in data structure and algorithms using Python; Paper Presentation on 'Biometric Technology'; Attended a 2-day Seminar on 'AI+ML'; Projects: IPL Data analysis using Machine Learning, Home Automation embedded system project, Dynamic Portfolio Website.</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>